<commit_message>
updated CI list and added new CIs
</commit_message>
<xml_diff>
--- a/Lhub_CIList_V1.xlsx
+++ b/Lhub_CIList_V1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Farah\Desktop\V1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\Project management\Learning-hub project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="50">
   <si>
     <t>CI ID</t>
   </si>
@@ -120,6 +120,60 @@
   </si>
   <si>
     <t>Project timeline</t>
+  </si>
+  <si>
+    <t>Lhub_CI_13</t>
+  </si>
+  <si>
+    <t>Lhub_CI_14</t>
+  </si>
+  <si>
+    <t>Lhub_CI_15</t>
+  </si>
+  <si>
+    <t>Lhub_CI_16</t>
+  </si>
+  <si>
+    <t>ERD</t>
+  </si>
+  <si>
+    <t>use case diagram</t>
+  </si>
+  <si>
+    <t>class diagram</t>
+  </si>
+  <si>
+    <t>sequence diagram</t>
+  </si>
+  <si>
+    <t>Lhub_CI_17</t>
+  </si>
+  <si>
+    <t>Lhub_CI_18</t>
+  </si>
+  <si>
+    <t>data flow diagram</t>
+  </si>
+  <si>
+    <t>high level diagram</t>
+  </si>
+  <si>
+    <t>Lhub_CI_19</t>
+  </si>
+  <si>
+    <t>Lhub_CI_20</t>
+  </si>
+  <si>
+    <t>Lhub_CI_21</t>
+  </si>
+  <si>
+    <t>hight level design document</t>
+  </si>
+  <si>
+    <t>wire frame</t>
+  </si>
+  <si>
+    <t>design PR sheet</t>
   </si>
 </sst>
 </file>
@@ -164,7 +218,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -187,22 +241,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -217,9 +260,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -502,16 +542,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:EU13"/>
+  <dimension ref="A1:EU22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.7109375" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" customWidth="1"/>
+    <col min="2" max="2" width="47.140625" customWidth="1"/>
     <col min="3" max="3" width="22.7109375" customWidth="1"/>
     <col min="4" max="4" width="19.5703125" customWidth="1"/>
     <col min="5" max="5" width="22.7109375" customWidth="1"/>
@@ -836,7 +876,7 @@
       <c r="A13" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>31</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -845,13 +885,109 @@
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
     </row>
+    <row r="14" spans="1:151" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:151" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:151" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15">
-      <formula1>$C$11:$C$13</formula1>
-    </dataValidation>
+  <dataValidations count="2">
     <dataValidation showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="C1"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C22">
       <formula1>$Q$8:$Q$10</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>